<commit_message>
Commited - GK - 21st Oct
</commit_message>
<xml_diff>
--- a/driverScript/Default.xlsx
+++ b/driverScript/Default.xlsx
@@ -183,10 +183,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="283845"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>

</xml_diff>

<commit_message>
Prakhar Neema : AR code changes
</commit_message>
<xml_diff>
--- a/driverScript/Default.xlsx
+++ b/driverScript/Default.xlsx
@@ -183,10 +183,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="283845"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>

</xml_diff>

<commit_message>
Associating iExpense library with the Driver script
</commit_message>
<xml_diff>
--- a/driverScript/Default.xlsx
+++ b/driverScript/Default.xlsx
@@ -183,10 +183,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="283845"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>

</xml_diff>

<commit_message>
12_nov-21 : Iproc merger of test cases
</commit_message>
<xml_diff>
--- a/driverScript/Default.xlsx
+++ b/driverScript/Default.xlsx
@@ -183,10 +183,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="283845"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>

</xml_diff>